<commit_message>
Gives selection to get the data in element-wise or surface-wise
</commit_message>
<xml_diff>
--- a/porosity_data_sample_1_1.xlsx
+++ b/porosity_data_sample_1_1.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BX3"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,9 +440,36 @@
           <t>0.3095 %</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>0.2059 %</t>
+        </is>
+      </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ebene 2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6.1089 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ebene 3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2.4272 %</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>

</xml_diff>

<commit_message>
Updates porosity data in the Excel file
</commit_message>
<xml_diff>
--- a/porosity_data_sample_1_1.xlsx
+++ b/porosity_data_sample_1_1.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:BX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,366 @@
           <t>0.2059 %</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>0.1951 %</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>0.2102 %</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>0.2518 %</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>0.2323 %</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>0.2352 %</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>0.2705 %</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>0.2593 %</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>0.2717 %</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>0.2655 %</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>0.3268 %</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>0.339 %</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>0.3311 %</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>0.3221 %</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>0.3653 %</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>0.3743 %</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>0.3716 %</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>0.3706 %</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>0.3828 %</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>0.3886 %</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>0.3881 %</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>0.3852 %</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>0.3773 %</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>0.3785 %</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>0.3726 %</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>0.3684 %</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>0.3688 %</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>0.3717 %</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>0.3663 %</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>0.3674 %</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>0.3626 %</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>0.3614 %</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>0.3601 %</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>0.3571 %</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>0.3556 %</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>0.3561 %</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>0.3549 %</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>0.3564 %</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>0.3549 %</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>0.3536 %</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>0.3563 %</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>0.3578 %</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>0.3588 %</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>0.3583 %</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>0.3564 %</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>0.3543 %</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>0.3635 %</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>0.3621 %</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>0.3585 %</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>0.3564 %</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>0.3573 %</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>0.3568 %</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
+          <t>0.3533 %</t>
+        </is>
+      </c>
+      <c r="BE1" t="inlineStr">
+        <is>
+          <t>0.3522 %</t>
+        </is>
+      </c>
+      <c r="BF1" t="inlineStr">
+        <is>
+          <t>0.3573 %</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>0.355 %</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>0.3528 %</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>0.3637 %</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>0.3717 %</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
+          <t>0.3708 %</t>
+        </is>
+      </c>
+      <c r="BL1" t="inlineStr">
+        <is>
+          <t>0.3724 %</t>
+        </is>
+      </c>
+      <c r="BM1" t="inlineStr">
+        <is>
+          <t>0.3906 %</t>
+        </is>
+      </c>
+      <c r="BN1" t="inlineStr">
+        <is>
+          <t>0.3882 %</t>
+        </is>
+      </c>
+      <c r="BO1" t="inlineStr">
+        <is>
+          <t>0.387 %</t>
+        </is>
+      </c>
+      <c r="BP1" t="inlineStr">
+        <is>
+          <t>0.4011 %</t>
+        </is>
+      </c>
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>0.4065 %</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
+          <t>0.4047 %</t>
+        </is>
+      </c>
+      <c r="BS1" t="inlineStr">
+        <is>
+          <t>0.4054 %</t>
+        </is>
+      </c>
+      <c r="BT1" t="inlineStr">
+        <is>
+          <t>0.4117 %</t>
+        </is>
+      </c>
+      <c r="BU1" t="inlineStr">
+        <is>
+          <t>0.4134 %</t>
+        </is>
+      </c>
+      <c r="BV1" t="inlineStr">
+        <is>
+          <t>0.4106 %</t>
+        </is>
+      </c>
+      <c r="BW1" t="inlineStr">
+        <is>
+          <t>0.4093 %</t>
+        </is>
+      </c>
+      <c r="BX1" t="inlineStr">
+        <is>
+          <t>0.4293 %</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" t="inlineStr">
@@ -457,6 +817,231 @@
           <t>6.1089 %</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1.7124 %</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.8997 %</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.6155 %</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.5285 %</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.5217 %</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.4764 %</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.4337 %</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.4608 %</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.4625 %</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0.4964 %</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0.5508 %</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0.5795 %</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0.6118 %</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0.6025 %</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0.6354 %</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0.6512 %</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0.6568 %</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0.663 %</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0.6628 %</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0.6693 %</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>0.661 %</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>0.6482 %</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0.6364 %</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>0.629 %</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>0.6135 %</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>0.6018 %</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>0.5988 %</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>0.5966 %</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>0.5861 %</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0.5742 %</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>0.5613 %</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>0.5597 %</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>0.5496 %</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>0.5366 %</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>0.5256 %</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>0.5176 %</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>0.5078 %</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>0.4988 %</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>0.4899 %</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>0.48 %</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>0.4744 %</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>0.465 %</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>0.4611 %</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>0.4554 %</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>0.4537 %</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
@@ -467,6 +1052,241 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>2.4272 %</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1.1154 %</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.6162 %</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.4351 %</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.3402 %</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.2684 %</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.2372 %</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.2117 %</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.1837 %</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0.1629 %</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0.1449 %</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0.1371 %</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>0.1256 %</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0.1155 %</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.1063 %</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0.1008 %</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0.0942 %</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0.0926 %</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>0.0902 %</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0.0922 %</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>0.0984 %</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>0.1087 %</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>0.123 %</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>0.1409 %</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.1587 %</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>0.1739 %</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>0.1897 %</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>0.1979 %</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>0.215 %</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>0.2329 %</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>0.2457 %</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>0.257 %</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>0.2662 %</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>0.2755 %</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>0.286 %</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>0.2941 %</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>0.3001 %</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>0.3051 %</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>0.3107 %</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>0.3177 %</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>0.3278 %</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>0.3565 %</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>0.3914 %</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>0.4142 %</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>0.4245 %</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>0.4337 %</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>0.4389 %</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>0.4421 %</t>
         </is>
       </c>
     </row>

</xml_diff>